<commit_message>
feat: import asset data by excel
</commit_message>
<xml_diff>
--- a/public/templates/asset-import-template.xlsx
+++ b/public/templates/asset-import-template.xlsx
@@ -3,19 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EDCF30B5-7AF0-434C-BC35-5322C27DC5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B769840E-EEC8-3149-90F5-E494012CCA81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="33600" windowHeight="19420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assets" sheetId="1" r:id="rId1"/>
+    <sheet name="Notes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
   <si>
     <t>Asset Name</t>
   </si>
@@ -44,9 +45,6 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>(example) Macbook Air M1 2020</t>
   </si>
   <si>
@@ -66,9 +64,6 @@
   </si>
   <si>
     <t>Product Management</t>
-  </si>
-  <si>
-    <t>active</t>
   </si>
   <si>
     <t xml:space="preserve">(example) VGA ASUS GT1030 2GB </t>
@@ -181,8 +176,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="&quot;Rp&quot;#,##0"/>
-    <numFmt numFmtId="172" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="&quot;Rp&quot;#,##0"/>
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -249,13 +244,16 @@
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -264,9 +262,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S213"/>
+  <dimension ref="A1:M213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -621,19 +616,17 @@
     <col min="9" max="9" width="15" customWidth="1"/>
     <col min="10" max="10" width="19" customWidth="1"/>
     <col min="11" max="13" width="25" customWidth="1"/>
-    <col min="14" max="14" width="15" customWidth="1"/>
-    <col min="16" max="16" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -657,240 +650,172 @@
         <v>7</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>8</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="N1" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="I2" s="2">
         <v>10500000</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="I3" s="2">
         <v>2540540</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N3" s="1" t="s">
+      <c r="D4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
         <v>27</v>
       </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="G4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="F4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="I4" s="2">
         <v>4211712</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I5" s="2"/>
       <c r="K5" s="1"/>
-      <c r="P5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q5" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I6" s="2"/>
       <c r="K6" s="1"/>
-      <c r="P6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q6" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I7" s="2"/>
       <c r="K7" s="1"/>
-      <c r="P7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q7" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I8" s="2"/>
       <c r="K8" s="1"/>
-      <c r="P8" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q8" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I9" s="2"/>
       <c r="K9" s="1"/>
-      <c r="P9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q9" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="R9" s="9"/>
-      <c r="S9" s="9"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I10" s="2"/>
       <c r="K10" s="1"/>
-      <c r="P10" s="1"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I11" s="2"/>
       <c r="K11" s="1"/>
-      <c r="P11" s="1"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I12" s="2"/>
       <c r="K12" s="1"/>
-      <c r="P12" s="1"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I13" s="2"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I14" s="2"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I15" s="2"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I16" s="2"/>
       <c r="K16" s="1"/>
     </row>
@@ -1492,19 +1417,109 @@
       <c r="K213" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="Q8:S8"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
   <ignoredErrors>
-    <ignoredError sqref="M2 M4 K2 P5:P7" numberStoredAsText="1"/>
+    <ignoredError sqref="M2 M4 K2" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FBC3586-2DC7-4A41-A241-A12FC4FB794D}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A5:A7" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>